<commit_message>
movie test script code updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -113,6 +113,39 @@
   </si>
   <si>
     <t>Element must be set</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//span[normalize-space()='Mumbai']"}
+  (Session info: MicrosoftEdge=143.0.3650.139)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
+Build info: version: '4.39.0', revision: '126f156aee'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Command: [e08981945b667b82685441a8e98fd2b0, findElement {using=xpath, value=//span[normalize-space()='Mumbai']}]
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 143.0.3650.139, fedcm:accounts: true, goog:processID: 15332, ms:edgeOptions: {debuggerAddress: localhost:49312}, msedge: {msedgedriverVersion: 143.0.3650.139 (30ed6d0ef65..., userDataDir: C:\Users\Dell\AppData\Local...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:49312/devtoo..., se:cdpVersion: 143.0.3650.139, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: e08981945b667b82685441a8e98fd2b0</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//span[normalize-space()='Mumbai']"}
+  (Session info: MicrosoftEdge=143.0.3650.139)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
+Build info: version: '4.39.0', revision: '126f156aee'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Command: [dd60e7e586cae05a60a2e0d0a4df4c1f, findElement {using=xpath, value=//span[normalize-space()='Mumbai']}]
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 143.0.3650.139, fedcm:accounts: true, goog:processID: 11864, ms:edgeOptions: {debuggerAddress: localhost:51599}, msedge: {msedgedriverVersion: 143.0.3650.139 (30ed6d0ef65..., userDataDir: C:\Users\Dell\AppData\Local...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:51599/devtoo..., se:cdpVersion: 143.0.3650.139, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: dd60e7e586cae05a60a2e0d0a4df4c1f</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//span[normalize-space()='Mumbai']"}
+  (Session info: MicrosoftEdge=143.0.3650.139)
+For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
+Build info: version: '4.39.0', revision: '126f156aee'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.7'
+Driver info: org.openqa.selenium.edge.EdgeDriver
+Command: [a3e3f7150133d13d23f4d814c433d495, findElement {using=xpath, value=//span[normalize-space()='Mumbai']}]
+Capabilities {acceptInsecureCerts: false, browserName: MicrosoftEdge, browserVersion: 143.0.3650.139, fedcm:accounts: true, goog:processID: 12132, ms:edgeOptions: {debuggerAddress: localhost:50459}, msedge: {msedgedriverVersion: 143.0.3650.139 (30ed6d0ef65..., userDataDir: C:\Users\Dell\AppData\Local...}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:50459/devtoo..., se:cdpVersion: 143.0.3650.139, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a3e3f7150133d13d23f4d814c433d495</t>
   </si>
 </sst>
 </file>

</xml_diff>